<commit_message>
Added POM Implementation of @Locator
</commit_message>
<xml_diff>
--- a/Cypress Codes.xlsx
+++ b/Cypress Codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashv\CypressAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE481E6-9D8A-4BAE-AC25-00FDE3DDDEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DEFD55-01BA-4424-A3E5-A9A3598A206D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{8064BC96-A7A6-451F-AE28-DFBAA5FECEEA}"/>
+    <workbookView xWindow="7200" yWindow="2160" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{8064BC96-A7A6-451F-AE28-DFBAA5FECEEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t xml:space="preserve">Selenium </t>
   </si>
@@ -92,13 +92,25 @@
   </si>
   <si>
     <t>Cypress is async</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POM </t>
+  </si>
+  <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>Cy.get('tag.classname').as('locator')</t>
+  </si>
+  <si>
+    <t>cy.get('@locator')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,16 +118,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -123,12 +149,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73372F3F-B1C5-4619-8FE2-0E3207FADFF9}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,21 +552,29 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
+      <c r="J2" s="2"/>
+      <c r="K2" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="K3" t="s">
+      <c r="I3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -497,31 +582,27 @@
       <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="I4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" t="s">
-        <v>7</v>
-      </c>
+      <c r="I4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="I5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I6" t="s">
+      <c r="I5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J5" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L7" t="s">
@@ -534,23 +615,48 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2659FBC3-0782-4819-990A-A4B1A7DDAA39}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>